<commit_message>
Update data and code for May 2022 baseline
</commit_message>
<xml_diff>
--- a/captax/data/outputs/Current-Law/comprehensive/supplemental_table_EMTRs_Current-Law_comprehensive.xlsx
+++ b/captax/data/outputs/Current-Law/comprehensive/supplemental_table_EMTRs_Current-Law_comprehensive.xlsx
@@ -510,37 +510,37 @@
     </row>
     <row r="9" spans="1:12">
       <c r="B9" s="5">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C9" s="5">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="D9" s="5">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="E9" s="5">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="F9" s="5">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="G9" s="5">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="H9" s="5">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="I9" s="5">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="J9" s="5">
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="K9" s="5">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="L9" s="5">
-        <v>2031</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -567,37 +567,37 @@
         <v>3</v>
       </c>
       <c r="B12" s="1">
-        <v>13</v>
+        <v>13.83</v>
       </c>
       <c r="C12" s="1">
-        <v>14.1</v>
+        <v>14.25</v>
       </c>
       <c r="D12" s="1">
-        <v>14.57</v>
+        <v>14.81</v>
       </c>
       <c r="E12" s="1">
-        <v>15.07</v>
+        <v>15.08</v>
       </c>
       <c r="F12" s="1">
-        <v>15.58</v>
+        <v>15.36</v>
       </c>
       <c r="G12" s="1">
-        <v>15.5</v>
+        <v>15.86</v>
       </c>
       <c r="H12" s="1">
-        <v>16.01</v>
+        <v>15.93</v>
       </c>
       <c r="I12" s="1">
-        <v>16.09</v>
+        <v>15.9</v>
       </c>
       <c r="J12" s="1">
-        <v>16.17</v>
+        <v>16</v>
       </c>
       <c r="K12" s="1">
-        <v>16.2</v>
+        <v>15.95</v>
       </c>
       <c r="L12" s="1">
-        <v>16.19</v>
+        <v>16.08</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -605,37 +605,37 @@
         <v>4</v>
       </c>
       <c r="B14" s="1">
-        <v>15.72</v>
+        <v>17.32</v>
       </c>
       <c r="C14" s="1">
-        <v>17.25</v>
+        <v>17.97</v>
       </c>
       <c r="D14" s="1">
-        <v>17.93</v>
+        <v>18.86</v>
       </c>
       <c r="E14" s="1">
-        <v>18.79</v>
+        <v>19.53</v>
       </c>
       <c r="F14" s="1">
-        <v>19.64</v>
+        <v>22.44</v>
       </c>
       <c r="G14" s="1">
-        <v>22.72</v>
+        <v>23.15</v>
       </c>
       <c r="H14" s="1">
-        <v>23.46</v>
+        <v>23.24</v>
       </c>
       <c r="I14" s="1">
-        <v>23.54</v>
+        <v>23.21</v>
       </c>
       <c r="J14" s="1">
-        <v>23.62</v>
+        <v>23.32</v>
       </c>
       <c r="K14" s="1">
-        <v>23.64</v>
+        <v>23.29</v>
       </c>
       <c r="L14" s="1">
-        <v>23.66</v>
+        <v>23.42</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -648,37 +648,37 @@
         <v>6</v>
       </c>
       <c r="B16" s="1">
-        <v>6.06</v>
+        <v>6.59</v>
       </c>
       <c r="C16" s="1">
-        <v>6.67</v>
+        <v>9.050000000000001</v>
       </c>
       <c r="D16" s="1">
-        <v>9.33</v>
+        <v>11.61</v>
       </c>
       <c r="E16" s="1">
-        <v>11.94</v>
+        <v>13.88</v>
       </c>
       <c r="F16" s="1">
-        <v>14.44</v>
+        <v>17.21</v>
       </c>
       <c r="G16" s="1">
-        <v>17.71</v>
+        <v>19.46</v>
       </c>
       <c r="H16" s="1">
-        <v>20.01</v>
+        <v>19.57</v>
       </c>
       <c r="I16" s="1">
-        <v>20.12</v>
+        <v>19.54</v>
       </c>
       <c r="J16" s="1">
-        <v>20.21</v>
+        <v>19.65</v>
       </c>
       <c r="K16" s="1">
-        <v>20.25</v>
+        <v>19.62</v>
       </c>
       <c r="L16" s="1">
-        <v>20.28</v>
+        <v>19.77</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -686,37 +686,37 @@
         <v>7</v>
       </c>
       <c r="B17" s="1">
-        <v>19.5</v>
+        <v>19.8</v>
       </c>
       <c r="C17" s="1">
-        <v>19.84</v>
+        <v>20.09</v>
       </c>
       <c r="D17" s="1">
-        <v>20.16</v>
+        <v>20.66</v>
       </c>
       <c r="E17" s="1">
-        <v>20.7</v>
+        <v>20.96</v>
       </c>
       <c r="F17" s="1">
-        <v>21.18</v>
+        <v>23.19</v>
       </c>
       <c r="G17" s="1">
-        <v>23.49</v>
+        <v>23.56</v>
       </c>
       <c r="H17" s="1">
-        <v>23.87</v>
+        <v>23.66</v>
       </c>
       <c r="I17" s="1">
-        <v>23.97</v>
+        <v>23.64</v>
       </c>
       <c r="J17" s="1">
-        <v>24.05</v>
+        <v>23.74</v>
       </c>
       <c r="K17" s="1">
-        <v>24.07</v>
+        <v>23.71</v>
       </c>
       <c r="L17" s="1">
-        <v>24.1</v>
+        <v>23.85</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -724,37 +724,37 @@
         <v>8</v>
       </c>
       <c r="B18" s="1">
-        <v>24.84</v>
+        <v>25.02</v>
       </c>
       <c r="C18" s="1">
-        <v>24.81</v>
+        <v>25.02</v>
       </c>
       <c r="D18" s="1">
-        <v>24.66</v>
+        <v>25.22</v>
       </c>
       <c r="E18" s="1">
-        <v>24.72</v>
+        <v>25.2</v>
       </c>
       <c r="F18" s="1">
-        <v>24.83</v>
+        <v>29.47</v>
       </c>
       <c r="G18" s="1">
+        <v>29.48</v>
+      </c>
+      <c r="H18" s="1">
+        <v>29.54</v>
+      </c>
+      <c r="I18" s="1">
+        <v>29.51</v>
+      </c>
+      <c r="J18" s="1">
+        <v>29.61</v>
+      </c>
+      <c r="K18" s="1">
         <v>29.59</v>
       </c>
-      <c r="H18" s="1">
-        <v>29.63</v>
-      </c>
-      <c r="I18" s="1">
-        <v>29.66</v>
-      </c>
-      <c r="J18" s="1">
-        <v>29.73</v>
-      </c>
-      <c r="K18" s="1">
-        <v>29.73</v>
-      </c>
       <c r="L18" s="1">
-        <v>29.73</v>
+        <v>29.7</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -762,37 +762,37 @@
         <v>9</v>
       </c>
       <c r="B19" s="1">
-        <v>-46.46</v>
+        <v>-6.56</v>
       </c>
       <c r="C19" s="1">
-        <v>-9.300000000000001</v>
+        <v>-6.76</v>
       </c>
       <c r="D19" s="1">
-        <v>-9.42</v>
+        <v>-6.7</v>
       </c>
       <c r="E19" s="1">
-        <v>-9.34</v>
+        <v>-6.84</v>
       </c>
       <c r="F19" s="1">
-        <v>-9.23</v>
+        <v>-5.21</v>
       </c>
       <c r="G19" s="1">
-        <v>-7.44</v>
+        <v>-5.26</v>
       </c>
       <c r="H19" s="1">
-        <v>-7.47</v>
+        <v>-5.12</v>
       </c>
       <c r="I19" s="1">
-        <v>-7.32</v>
+        <v>-5.15</v>
       </c>
       <c r="J19" s="1">
-        <v>-7.21</v>
+        <v>-5.02</v>
       </c>
       <c r="K19" s="1">
-        <v>-7.17</v>
+        <v>-5.06</v>
       </c>
       <c r="L19" s="1">
-        <v>-7.12</v>
+        <v>-4.88</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -800,37 +800,37 @@
         <v>10</v>
       </c>
       <c r="B20" s="1">
-        <v>7.41</v>
+        <v>7.87</v>
       </c>
       <c r="C20" s="1">
-        <v>7.93</v>
+        <v>12.05</v>
       </c>
       <c r="D20" s="1">
-        <v>12.4</v>
+        <v>16.1</v>
       </c>
       <c r="E20" s="1">
-        <v>16.57</v>
+        <v>19.63</v>
       </c>
       <c r="F20" s="1">
-        <v>20.41</v>
+        <v>23.86</v>
       </c>
       <c r="G20" s="1">
-        <v>24.59</v>
+        <v>26.91</v>
       </c>
       <c r="H20" s="1">
-        <v>27.72</v>
+        <v>27.03</v>
       </c>
       <c r="I20" s="1">
-        <v>27.84</v>
+        <v>27.01</v>
       </c>
       <c r="J20" s="1">
-        <v>27.94</v>
+        <v>27.12</v>
       </c>
       <c r="K20" s="1">
-        <v>27.99</v>
+        <v>27.09</v>
       </c>
       <c r="L20" s="1">
-        <v>28.02</v>
+        <v>27.24</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -838,37 +838,37 @@
         <v>11</v>
       </c>
       <c r="B21" s="1">
-        <v>30.16</v>
+        <v>29.84</v>
       </c>
       <c r="C21" s="1">
-        <v>30.2</v>
+        <v>29.75</v>
       </c>
       <c r="D21" s="1">
-        <v>30.01</v>
+        <v>29.85</v>
       </c>
       <c r="E21" s="1">
-        <v>30.06</v>
+        <v>29.82</v>
       </c>
       <c r="F21" s="1">
-        <v>30.13</v>
+        <v>32.7</v>
       </c>
       <c r="G21" s="1">
-        <v>33.42</v>
+        <v>32.68</v>
       </c>
       <c r="H21" s="1">
-        <v>33.45</v>
+        <v>32.75</v>
       </c>
       <c r="I21" s="1">
-        <v>33.49</v>
+        <v>32.71</v>
       </c>
       <c r="J21" s="1">
-        <v>33.53</v>
+        <v>32.79</v>
       </c>
       <c r="K21" s="1">
-        <v>33.53</v>
+        <v>32.77</v>
       </c>
       <c r="L21" s="1">
-        <v>33.54</v>
+        <v>32.86</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -881,37 +881,37 @@
         <v>13</v>
       </c>
       <c r="B23" s="1">
-        <v>17.99</v>
+        <v>19.18</v>
       </c>
       <c r="C23" s="1">
-        <v>19.21</v>
+        <v>19.9</v>
       </c>
       <c r="D23" s="1">
-        <v>19.78</v>
+        <v>20.74</v>
       </c>
       <c r="E23" s="1">
-        <v>20.57</v>
+        <v>21.46</v>
       </c>
       <c r="F23" s="1">
-        <v>21.3</v>
+        <v>24.47</v>
       </c>
       <c r="G23" s="1">
-        <v>24.74</v>
+        <v>25.17</v>
       </c>
       <c r="H23" s="1">
-        <v>25.47</v>
+        <v>25.22</v>
       </c>
       <c r="I23" s="1">
-        <v>25.5</v>
+        <v>25.18</v>
       </c>
       <c r="J23" s="1">
-        <v>25.49</v>
+        <v>25.23</v>
       </c>
       <c r="K23" s="1">
-        <v>25.46</v>
+        <v>25.21</v>
       </c>
       <c r="L23" s="1">
-        <v>25.47</v>
+        <v>25.26</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -919,37 +919,37 @@
         <v>14</v>
       </c>
       <c r="B24" s="1">
-        <v>2.48</v>
+        <v>7.7</v>
       </c>
       <c r="C24" s="1">
-        <v>6.05</v>
+        <v>8.050000000000001</v>
       </c>
       <c r="D24" s="1">
-        <v>7.44</v>
+        <v>9.17</v>
       </c>
       <c r="E24" s="1">
-        <v>8.779999999999999</v>
+        <v>9.470000000000001</v>
       </c>
       <c r="F24" s="1">
-        <v>10.29</v>
+        <v>11.32</v>
       </c>
       <c r="G24" s="1">
-        <v>10.6</v>
+        <v>12.06</v>
       </c>
       <c r="H24" s="1">
-        <v>11.39</v>
+        <v>12.43</v>
       </c>
       <c r="I24" s="1">
-        <v>11.84</v>
+        <v>12.45</v>
       </c>
       <c r="J24" s="1">
-        <v>12.44</v>
+        <v>12.88</v>
       </c>
       <c r="K24" s="1">
-        <v>12.79</v>
+        <v>12.81</v>
       </c>
       <c r="L24" s="1">
-        <v>12.89</v>
+        <v>13.4</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -962,37 +962,37 @@
         <v>16</v>
       </c>
       <c r="B26" s="1">
-        <v>13.55</v>
+        <v>15.62</v>
       </c>
       <c r="C26" s="1">
-        <v>15.64</v>
+        <v>16.32</v>
       </c>
       <c r="D26" s="1">
-        <v>16.47</v>
+        <v>17.26</v>
       </c>
       <c r="E26" s="1">
-        <v>17.46</v>
+        <v>17.98</v>
       </c>
       <c r="F26" s="1">
-        <v>18.41</v>
+        <v>19.44</v>
       </c>
       <c r="G26" s="1">
-        <v>19.77</v>
+        <v>20.19</v>
       </c>
       <c r="H26" s="1">
-        <v>20.54</v>
+        <v>20.32</v>
       </c>
       <c r="I26" s="1">
-        <v>20.68</v>
+        <v>20.29</v>
       </c>
       <c r="J26" s="1">
-        <v>20.77</v>
+        <v>20.4</v>
       </c>
       <c r="K26" s="1">
-        <v>20.81</v>
+        <v>20.36</v>
       </c>
       <c r="L26" s="1">
-        <v>20.85</v>
+        <v>20.51</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1000,37 +1000,37 @@
         <v>17</v>
       </c>
       <c r="B27" s="1">
-        <v>20.39</v>
+        <v>21.04</v>
       </c>
       <c r="C27" s="1">
-        <v>20.78</v>
+        <v>21.6</v>
       </c>
       <c r="D27" s="1">
-        <v>21.15</v>
+        <v>22.38</v>
       </c>
       <c r="E27" s="1">
-        <v>21.74</v>
+        <v>22.91</v>
       </c>
       <c r="F27" s="1">
-        <v>22.37</v>
+        <v>28.65</v>
       </c>
       <c r="G27" s="1">
-        <v>28.84</v>
+        <v>29.27</v>
       </c>
       <c r="H27" s="1">
-        <v>29.5</v>
+        <v>29.31</v>
       </c>
       <c r="I27" s="1">
-        <v>29.51</v>
+        <v>29.27</v>
       </c>
       <c r="J27" s="1">
-        <v>29.56</v>
+        <v>29.37</v>
       </c>
       <c r="K27" s="1">
-        <v>29.54</v>
+        <v>29.36</v>
       </c>
       <c r="L27" s="1">
-        <v>29.53</v>
+        <v>29.45</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1038,37 +1038,37 @@
         <v>18</v>
       </c>
       <c r="B29" s="1">
-        <v>7.55</v>
+        <v>6.71</v>
       </c>
       <c r="C29" s="1">
-        <v>7.69</v>
+        <v>6.58</v>
       </c>
       <c r="D29" s="1">
-        <v>7.67</v>
+        <v>6.35</v>
       </c>
       <c r="E29" s="1">
-        <v>7.35</v>
+        <v>5.66</v>
       </c>
       <c r="F29" s="1">
-        <v>7.04</v>
+        <v>-1.42</v>
       </c>
       <c r="G29" s="1">
-        <v>-1.86</v>
+        <v>-1.61</v>
       </c>
       <c r="H29" s="1">
-        <v>-2.1</v>
+        <v>-1.6</v>
       </c>
       <c r="I29" s="1">
-        <v>-2.06</v>
+        <v>-1.65</v>
       </c>
       <c r="J29" s="1">
-        <v>-2</v>
+        <v>-1.58</v>
       </c>
       <c r="K29" s="1">
-        <v>-1.97</v>
+        <v>-1.68</v>
       </c>
       <c r="L29" s="1">
-        <v>-2.04</v>
+        <v>-1.58</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1081,37 +1081,37 @@
         <v>13</v>
       </c>
       <c r="B31" s="1">
-        <v>-0.28</v>
+        <v>-0.26</v>
       </c>
       <c r="C31" s="1">
-        <v>-0.26</v>
+        <v>-0.23</v>
       </c>
       <c r="D31" s="1">
         <v>-0.24</v>
       </c>
       <c r="E31" s="1">
-        <v>-0.24</v>
+        <v>-0.26</v>
       </c>
       <c r="F31" s="1">
-        <v>-0.25</v>
+        <v>-3.13</v>
       </c>
       <c r="G31" s="1">
-        <v>-3.5</v>
+        <v>-3.17</v>
       </c>
       <c r="H31" s="1">
-        <v>-3.58</v>
+        <v>-3.16</v>
       </c>
       <c r="I31" s="1">
-        <v>-3.59</v>
+        <v>-3.16</v>
       </c>
       <c r="J31" s="1">
-        <v>-3.61</v>
+        <v>-3.17</v>
       </c>
       <c r="K31" s="1">
-        <v>-3.6</v>
+        <v>-3.16</v>
       </c>
       <c r="L31" s="1">
-        <v>-3.61</v>
+        <v>-3.16</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -1119,37 +1119,37 @@
         <v>14</v>
       </c>
       <c r="B32" s="1">
-        <v>29.62</v>
+        <v>25.42</v>
       </c>
       <c r="C32" s="1">
-        <v>29.94</v>
+        <v>24.82</v>
       </c>
       <c r="D32" s="1">
-        <v>29.78</v>
+        <v>24.25</v>
       </c>
       <c r="E32" s="1">
-        <v>28.77</v>
+        <v>22.07</v>
       </c>
       <c r="F32" s="1">
-        <v>27.94</v>
+        <v>4.53</v>
       </c>
       <c r="G32" s="1">
-        <v>4.41</v>
+        <v>3.82</v>
       </c>
       <c r="H32" s="1">
-        <v>3.56</v>
+        <v>3.84</v>
       </c>
       <c r="I32" s="1">
-        <v>3.83</v>
+        <v>3.63</v>
       </c>
       <c r="J32" s="1">
-        <v>4.17</v>
+        <v>3.96</v>
       </c>
       <c r="K32" s="1">
-        <v>4.33</v>
+        <v>3.49</v>
       </c>
       <c r="L32" s="1">
-        <v>4.02</v>
+        <v>3.98</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -1162,37 +1162,37 @@
         <v>20</v>
       </c>
       <c r="B35" s="1">
-        <v>13.95</v>
+        <v>14.49</v>
       </c>
       <c r="C35" s="1">
-        <v>14.78</v>
+        <v>14.77</v>
       </c>
       <c r="D35" s="1">
-        <v>15.1</v>
+        <v>15.18</v>
       </c>
       <c r="E35" s="1">
-        <v>15.43</v>
+        <v>15.28</v>
       </c>
       <c r="F35" s="1">
-        <v>15.78</v>
+        <v>15.21</v>
       </c>
       <c r="G35" s="1">
-        <v>15.27</v>
+        <v>15.55</v>
       </c>
       <c r="H35" s="1">
+        <v>15.62</v>
+      </c>
+      <c r="I35" s="1">
+        <v>15.58</v>
+      </c>
+      <c r="J35" s="1">
+        <v>15.68</v>
+      </c>
+      <c r="K35" s="1">
         <v>15.63</v>
       </c>
-      <c r="I35" s="1">
-        <v>15.7</v>
-      </c>
-      <c r="J35" s="1">
-        <v>15.78</v>
-      </c>
-      <c r="K35" s="1">
-        <v>15.8</v>
-      </c>
       <c r="L35" s="1">
-        <v>15.8</v>
+        <v>15.76</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -1200,37 +1200,37 @@
         <v>21</v>
       </c>
       <c r="B36" s="1">
-        <v>18</v>
+        <v>19.33</v>
       </c>
       <c r="C36" s="1">
-        <v>19.21</v>
+        <v>19.83</v>
       </c>
       <c r="D36" s="1">
-        <v>19.71</v>
+        <v>20.56</v>
       </c>
       <c r="E36" s="1">
-        <v>20.39</v>
+        <v>21.07</v>
       </c>
       <c r="F36" s="1">
-        <v>21.08</v>
+        <v>24.12</v>
       </c>
       <c r="G36" s="1">
-        <v>24.34</v>
+        <v>24.67</v>
       </c>
       <c r="H36" s="1">
-        <v>24.92</v>
+        <v>24.76</v>
       </c>
       <c r="I36" s="1">
-        <v>25</v>
+        <v>24.73</v>
       </c>
       <c r="J36" s="1">
-        <v>25.08</v>
+        <v>24.84</v>
       </c>
       <c r="K36" s="1">
-        <v>25.09</v>
+        <v>24.81</v>
       </c>
       <c r="L36" s="1">
-        <v>25.11</v>
+        <v>24.94</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -1238,37 +1238,37 @@
         <v>22</v>
       </c>
       <c r="B37" s="1">
-        <v>27.03</v>
+        <v>27.4</v>
       </c>
       <c r="C37" s="1">
-        <v>27.1</v>
+        <v>27.34</v>
       </c>
       <c r="D37" s="1">
-        <v>26.94</v>
+        <v>27.48</v>
       </c>
       <c r="E37" s="1">
-        <v>26.97</v>
+        <v>27.43</v>
       </c>
       <c r="F37" s="1">
-        <v>27.06</v>
+        <v>30.96</v>
       </c>
       <c r="G37" s="1">
-        <v>30.96</v>
+        <v>30.94</v>
       </c>
       <c r="H37" s="1">
-        <v>30.96</v>
+        <v>31.01</v>
       </c>
       <c r="I37" s="1">
-        <v>31.01</v>
+        <v>30.98</v>
       </c>
       <c r="J37" s="1">
         <v>31.08</v>
       </c>
       <c r="K37" s="1">
-        <v>31.08</v>
+        <v>31.06</v>
       </c>
       <c r="L37" s="1">
-        <v>31.1</v>
+        <v>31.17</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -1276,37 +1276,37 @@
         <v>23</v>
       </c>
       <c r="B38" s="1">
-        <v>7.55</v>
+        <v>6.71</v>
       </c>
       <c r="C38" s="1">
-        <v>7.69</v>
+        <v>6.58</v>
       </c>
       <c r="D38" s="1">
-        <v>7.67</v>
+        <v>6.35</v>
       </c>
       <c r="E38" s="1">
-        <v>7.35</v>
+        <v>5.66</v>
       </c>
       <c r="F38" s="1">
-        <v>7.04</v>
+        <v>-1.42</v>
       </c>
       <c r="G38" s="1">
-        <v>-1.86</v>
+        <v>-1.61</v>
       </c>
       <c r="H38" s="1">
-        <v>-2.1</v>
+        <v>-1.6</v>
       </c>
       <c r="I38" s="1">
-        <v>-2.06</v>
+        <v>-1.65</v>
       </c>
       <c r="J38" s="1">
-        <v>-2</v>
+        <v>-1.58</v>
       </c>
       <c r="K38" s="1">
-        <v>-1.97</v>
+        <v>-1.68</v>
       </c>
       <c r="L38" s="1">
-        <v>-2.04</v>
+        <v>-1.58</v>
       </c>
     </row>
     <row r="40" spans="1:12">

</xml_diff>

<commit_message>
Update data and code for February 2023 baseline
</commit_message>
<xml_diff>
--- a/captax/data/outputs/Current-Law/comprehensive/supplemental_table_EMTRs_Current-Law_comprehensive.xlsx
+++ b/captax/data/outputs/Current-Law/comprehensive/supplemental_table_EMTRs_Current-Law_comprehensive.xlsx
@@ -510,37 +510,37 @@
     </row>
     <row r="9" spans="1:12">
       <c r="B9" s="5">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C9" s="5">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="D9" s="5">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="E9" s="5">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="F9" s="5">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="G9" s="5">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="H9" s="5">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="I9" s="5">
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="J9" s="5">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="K9" s="5">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="L9" s="5">
-        <v>2032</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -567,37 +567,37 @@
         <v>3</v>
       </c>
       <c r="B12" s="1">
-        <v>13.83</v>
+        <v>15.28</v>
       </c>
       <c r="C12" s="1">
-        <v>14.25</v>
+        <v>15.63</v>
       </c>
       <c r="D12" s="1">
-        <v>14.81</v>
+        <v>15.74</v>
       </c>
       <c r="E12" s="1">
-        <v>15.08</v>
+        <v>15.62</v>
       </c>
       <c r="F12" s="1">
-        <v>15.36</v>
+        <v>16.44</v>
       </c>
       <c r="G12" s="1">
-        <v>15.86</v>
+        <v>16.46</v>
       </c>
       <c r="H12" s="1">
-        <v>15.93</v>
+        <v>16.24</v>
       </c>
       <c r="I12" s="1">
-        <v>15.9</v>
+        <v>16.26</v>
       </c>
       <c r="J12" s="1">
-        <v>16</v>
+        <v>16.23</v>
       </c>
       <c r="K12" s="1">
-        <v>15.95</v>
+        <v>16.32</v>
       </c>
       <c r="L12" s="1">
-        <v>16.08</v>
+        <v>16.49</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -605,37 +605,37 @@
         <v>4</v>
       </c>
       <c r="B14" s="1">
-        <v>17.32</v>
+        <v>18.84</v>
       </c>
       <c r="C14" s="1">
-        <v>17.97</v>
+        <v>19.47</v>
       </c>
       <c r="D14" s="1">
-        <v>18.86</v>
+        <v>19.9</v>
       </c>
       <c r="E14" s="1">
-        <v>19.53</v>
+        <v>22.55</v>
       </c>
       <c r="F14" s="1">
-        <v>22.44</v>
+        <v>23.6</v>
       </c>
       <c r="G14" s="1">
-        <v>23.15</v>
+        <v>23.66</v>
       </c>
       <c r="H14" s="1">
-        <v>23.24</v>
+        <v>23.52</v>
       </c>
       <c r="I14" s="1">
-        <v>23.21</v>
+        <v>23.56</v>
       </c>
       <c r="J14" s="1">
-        <v>23.32</v>
+        <v>23.58</v>
       </c>
       <c r="K14" s="1">
-        <v>23.29</v>
+        <v>23.71</v>
       </c>
       <c r="L14" s="1">
-        <v>23.42</v>
+        <v>23.9</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -648,37 +648,37 @@
         <v>6</v>
       </c>
       <c r="B16" s="1">
-        <v>6.59</v>
+        <v>9.84</v>
       </c>
       <c r="C16" s="1">
-        <v>9.050000000000001</v>
+        <v>12.12</v>
       </c>
       <c r="D16" s="1">
-        <v>11.61</v>
+        <v>14.27</v>
       </c>
       <c r="E16" s="1">
-        <v>13.88</v>
+        <v>17.2</v>
       </c>
       <c r="F16" s="1">
-        <v>17.21</v>
+        <v>20.28</v>
       </c>
       <c r="G16" s="1">
-        <v>19.46</v>
+        <v>20.35</v>
       </c>
       <c r="H16" s="1">
-        <v>19.57</v>
+        <v>20.21</v>
       </c>
       <c r="I16" s="1">
-        <v>19.54</v>
+        <v>20.25</v>
       </c>
       <c r="J16" s="1">
-        <v>19.65</v>
+        <v>20.27</v>
       </c>
       <c r="K16" s="1">
-        <v>19.62</v>
+        <v>20.38</v>
       </c>
       <c r="L16" s="1">
-        <v>19.77</v>
+        <v>20.57</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -686,37 +686,37 @@
         <v>7</v>
       </c>
       <c r="B17" s="1">
-        <v>19.8</v>
+        <v>21.02</v>
       </c>
       <c r="C17" s="1">
-        <v>20.09</v>
+        <v>21.27</v>
       </c>
       <c r="D17" s="1">
-        <v>20.66</v>
+        <v>21.27</v>
       </c>
       <c r="E17" s="1">
-        <v>20.96</v>
+        <v>23.22</v>
       </c>
       <c r="F17" s="1">
-        <v>23.19</v>
+        <v>23.88</v>
       </c>
       <c r="G17" s="1">
-        <v>23.56</v>
+        <v>23.94</v>
       </c>
       <c r="H17" s="1">
-        <v>23.66</v>
+        <v>23.81</v>
       </c>
       <c r="I17" s="1">
-        <v>23.64</v>
+        <v>23.85</v>
       </c>
       <c r="J17" s="1">
-        <v>23.74</v>
+        <v>23.87</v>
       </c>
       <c r="K17" s="1">
-        <v>23.71</v>
+        <v>23.99</v>
       </c>
       <c r="L17" s="1">
-        <v>23.85</v>
+        <v>24.18</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -724,37 +724,37 @@
         <v>8</v>
       </c>
       <c r="B18" s="1">
-        <v>25.02</v>
+        <v>25.29</v>
       </c>
       <c r="C18" s="1">
-        <v>25.02</v>
+        <v>25.38</v>
       </c>
       <c r="D18" s="1">
-        <v>25.22</v>
+        <v>25.09</v>
       </c>
       <c r="E18" s="1">
-        <v>25.2</v>
+        <v>29.2</v>
       </c>
       <c r="F18" s="1">
-        <v>29.47</v>
+        <v>29.39</v>
       </c>
       <c r="G18" s="1">
-        <v>29.48</v>
+        <v>29.41</v>
       </c>
       <c r="H18" s="1">
-        <v>29.54</v>
+        <v>29.25</v>
       </c>
       <c r="I18" s="1">
-        <v>29.51</v>
+        <v>29.31</v>
       </c>
       <c r="J18" s="1">
-        <v>29.61</v>
+        <v>29.31</v>
       </c>
       <c r="K18" s="1">
-        <v>29.59</v>
+        <v>29.46</v>
       </c>
       <c r="L18" s="1">
-        <v>29.7</v>
+        <v>29.64</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -762,37 +762,37 @@
         <v>9</v>
       </c>
       <c r="B19" s="1">
-        <v>-6.56</v>
+        <v>-4.93</v>
       </c>
       <c r="C19" s="1">
-        <v>-6.76</v>
+        <v>-5.16</v>
       </c>
       <c r="D19" s="1">
-        <v>-6.7</v>
+        <v>-5.39</v>
       </c>
       <c r="E19" s="1">
-        <v>-6.84</v>
+        <v>-4.14</v>
       </c>
       <c r="F19" s="1">
-        <v>-5.21</v>
+        <v>-4.09</v>
       </c>
       <c r="G19" s="1">
-        <v>-5.26</v>
+        <v>-3.98</v>
       </c>
       <c r="H19" s="1">
-        <v>-5.12</v>
+        <v>-4.14</v>
       </c>
       <c r="I19" s="1">
-        <v>-5.15</v>
+        <v>-4.06</v>
       </c>
       <c r="J19" s="1">
-        <v>-5.02</v>
+        <v>-3.98</v>
       </c>
       <c r="K19" s="1">
-        <v>-5.06</v>
+        <v>-3.78</v>
       </c>
       <c r="L19" s="1">
-        <v>-4.88</v>
+        <v>-3.5</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -800,37 +800,37 @@
         <v>10</v>
       </c>
       <c r="B20" s="1">
-        <v>7.87</v>
+        <v>14.52</v>
       </c>
       <c r="C20" s="1">
-        <v>12.05</v>
+        <v>18.13</v>
       </c>
       <c r="D20" s="1">
-        <v>16.1</v>
+        <v>21.45</v>
       </c>
       <c r="E20" s="1">
-        <v>19.63</v>
+        <v>25.17</v>
       </c>
       <c r="F20" s="1">
-        <v>23.86</v>
+        <v>28.21</v>
       </c>
       <c r="G20" s="1">
-        <v>26.91</v>
+        <v>28.28</v>
       </c>
       <c r="H20" s="1">
-        <v>27.03</v>
+        <v>28.15</v>
       </c>
       <c r="I20" s="1">
-        <v>27.01</v>
+        <v>28.18</v>
       </c>
       <c r="J20" s="1">
-        <v>27.12</v>
+        <v>28.2</v>
       </c>
       <c r="K20" s="1">
-        <v>27.09</v>
+        <v>28.31</v>
       </c>
       <c r="L20" s="1">
-        <v>27.24</v>
+        <v>28.5</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -838,37 +838,37 @@
         <v>11</v>
       </c>
       <c r="B21" s="1">
-        <v>29.84</v>
+        <v>30.6</v>
       </c>
       <c r="C21" s="1">
-        <v>29.75</v>
+        <v>30.54</v>
       </c>
       <c r="D21" s="1">
-        <v>29.85</v>
+        <v>30.33</v>
       </c>
       <c r="E21" s="1">
-        <v>29.82</v>
+        <v>33.15</v>
       </c>
       <c r="F21" s="1">
-        <v>32.7</v>
+        <v>33.26</v>
       </c>
       <c r="G21" s="1">
-        <v>32.68</v>
+        <v>33.31</v>
       </c>
       <c r="H21" s="1">
-        <v>32.75</v>
+        <v>33.2</v>
       </c>
       <c r="I21" s="1">
-        <v>32.71</v>
+        <v>33.24</v>
       </c>
       <c r="J21" s="1">
-        <v>32.79</v>
+        <v>33.26</v>
       </c>
       <c r="K21" s="1">
-        <v>32.77</v>
+        <v>33.39</v>
       </c>
       <c r="L21" s="1">
-        <v>32.86</v>
+        <v>33.55</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -881,37 +881,37 @@
         <v>13</v>
       </c>
       <c r="B23" s="1">
-        <v>19.18</v>
+        <v>20.94</v>
       </c>
       <c r="C23" s="1">
-        <v>19.9</v>
+        <v>21.57</v>
       </c>
       <c r="D23" s="1">
-        <v>20.74</v>
+        <v>22.07</v>
       </c>
       <c r="E23" s="1">
-        <v>21.46</v>
+        <v>25.16</v>
       </c>
       <c r="F23" s="1">
-        <v>24.47</v>
+        <v>26.15</v>
       </c>
       <c r="G23" s="1">
-        <v>25.17</v>
+        <v>26.21</v>
       </c>
       <c r="H23" s="1">
-        <v>25.22</v>
+        <v>26.14</v>
       </c>
       <c r="I23" s="1">
-        <v>25.18</v>
+        <v>26.15</v>
       </c>
       <c r="J23" s="1">
-        <v>25.23</v>
+        <v>26.17</v>
       </c>
       <c r="K23" s="1">
-        <v>25.21</v>
+        <v>26.27</v>
       </c>
       <c r="L23" s="1">
-        <v>25.26</v>
+        <v>26.37</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -919,37 +919,37 @@
         <v>14</v>
       </c>
       <c r="B24" s="1">
-        <v>7.7</v>
+        <v>9.59</v>
       </c>
       <c r="C24" s="1">
-        <v>8.050000000000001</v>
+        <v>10.26</v>
       </c>
       <c r="D24" s="1">
-        <v>9.17</v>
+        <v>10.34</v>
       </c>
       <c r="E24" s="1">
-        <v>9.470000000000001</v>
+        <v>10.29</v>
       </c>
       <c r="F24" s="1">
-        <v>11.32</v>
+        <v>11.57</v>
       </c>
       <c r="G24" s="1">
-        <v>12.06</v>
+        <v>11.63</v>
       </c>
       <c r="H24" s="1">
-        <v>12.43</v>
+        <v>11.19</v>
       </c>
       <c r="I24" s="1">
-        <v>12.45</v>
+        <v>11.41</v>
       </c>
       <c r="J24" s="1">
-        <v>12.88</v>
+        <v>11.44</v>
       </c>
       <c r="K24" s="1">
-        <v>12.81</v>
+        <v>11.74</v>
       </c>
       <c r="L24" s="1">
-        <v>13.4</v>
+        <v>12.37</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -962,37 +962,37 @@
         <v>16</v>
       </c>
       <c r="B26" s="1">
-        <v>15.62</v>
+        <v>17.58</v>
       </c>
       <c r="C26" s="1">
-        <v>16.32</v>
+        <v>18.2</v>
       </c>
       <c r="D26" s="1">
-        <v>17.26</v>
+        <v>18.76</v>
       </c>
       <c r="E26" s="1">
-        <v>17.98</v>
+        <v>19.88</v>
       </c>
       <c r="F26" s="1">
-        <v>19.44</v>
+        <v>21.04</v>
       </c>
       <c r="G26" s="1">
-        <v>20.19</v>
+        <v>21.13</v>
       </c>
       <c r="H26" s="1">
-        <v>20.32</v>
+        <v>21</v>
       </c>
       <c r="I26" s="1">
-        <v>20.29</v>
+        <v>21.03</v>
       </c>
       <c r="J26" s="1">
-        <v>20.4</v>
+        <v>21.06</v>
       </c>
       <c r="K26" s="1">
-        <v>20.36</v>
+        <v>21.17</v>
       </c>
       <c r="L26" s="1">
-        <v>20.51</v>
+        <v>21.36</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1000,37 +1000,37 @@
         <v>17</v>
       </c>
       <c r="B27" s="1">
-        <v>21.04</v>
+        <v>21.66</v>
       </c>
       <c r="C27" s="1">
-        <v>21.6</v>
+        <v>22.33</v>
       </c>
       <c r="D27" s="1">
-        <v>22.38</v>
+        <v>22.48</v>
       </c>
       <c r="E27" s="1">
-        <v>22.91</v>
+        <v>28.2</v>
       </c>
       <c r="F27" s="1">
-        <v>28.65</v>
+        <v>29.04</v>
       </c>
       <c r="G27" s="1">
-        <v>29.27</v>
+        <v>29.04</v>
       </c>
       <c r="H27" s="1">
-        <v>29.31</v>
+        <v>28.88</v>
       </c>
       <c r="I27" s="1">
-        <v>29.27</v>
+        <v>28.95</v>
       </c>
       <c r="J27" s="1">
-        <v>29.37</v>
+        <v>28.95</v>
       </c>
       <c r="K27" s="1">
-        <v>29.36</v>
+        <v>29.11</v>
       </c>
       <c r="L27" s="1">
-        <v>29.45</v>
+        <v>29.29</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1038,37 +1038,37 @@
         <v>18</v>
       </c>
       <c r="B29" s="1">
-        <v>6.71</v>
+        <v>7.98</v>
       </c>
       <c r="C29" s="1">
-        <v>6.58</v>
+        <v>7.65</v>
       </c>
       <c r="D29" s="1">
-        <v>6.35</v>
+        <v>6.99</v>
       </c>
       <c r="E29" s="1">
-        <v>5.66</v>
+        <v>-0.71</v>
       </c>
       <c r="F29" s="1">
-        <v>-1.42</v>
+        <v>-0.68</v>
       </c>
       <c r="G29" s="1">
-        <v>-1.61</v>
+        <v>-0.77</v>
       </c>
       <c r="H29" s="1">
-        <v>-1.6</v>
+        <v>-1.21</v>
       </c>
       <c r="I29" s="1">
-        <v>-1.65</v>
+        <v>-1.26</v>
       </c>
       <c r="J29" s="1">
-        <v>-1.58</v>
+        <v>-1.43</v>
       </c>
       <c r="K29" s="1">
-        <v>-1.68</v>
+        <v>-1.46</v>
       </c>
       <c r="L29" s="1">
-        <v>-1.58</v>
+        <v>-1.39</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1081,7 +1081,7 @@
         <v>13</v>
       </c>
       <c r="B31" s="1">
-        <v>-0.26</v>
+        <v>-0.23</v>
       </c>
       <c r="C31" s="1">
         <v>-0.23</v>
@@ -1090,28 +1090,28 @@
         <v>-0.24</v>
       </c>
       <c r="E31" s="1">
-        <v>-0.26</v>
+        <v>-3.32</v>
       </c>
       <c r="F31" s="1">
-        <v>-3.13</v>
+        <v>-3.38</v>
       </c>
       <c r="G31" s="1">
-        <v>-3.17</v>
+        <v>-3.38</v>
       </c>
       <c r="H31" s="1">
-        <v>-3.16</v>
+        <v>-3.37</v>
       </c>
       <c r="I31" s="1">
-        <v>-3.16</v>
+        <v>-3.37</v>
       </c>
       <c r="J31" s="1">
-        <v>-3.17</v>
+        <v>-3.37</v>
       </c>
       <c r="K31" s="1">
-        <v>-3.16</v>
+        <v>-3.37</v>
       </c>
       <c r="L31" s="1">
-        <v>-3.16</v>
+        <v>-3.37</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -1119,37 +1119,37 @@
         <v>14</v>
       </c>
       <c r="B32" s="1">
-        <v>25.42</v>
+        <v>26.85</v>
       </c>
       <c r="C32" s="1">
-        <v>24.82</v>
+        <v>26.01</v>
       </c>
       <c r="D32" s="1">
-        <v>24.25</v>
+        <v>24.12</v>
       </c>
       <c r="E32" s="1">
-        <v>22.07</v>
+        <v>6.87</v>
       </c>
       <c r="F32" s="1">
-        <v>4.53</v>
+        <v>7.19</v>
       </c>
       <c r="G32" s="1">
-        <v>3.82</v>
+        <v>6.85</v>
       </c>
       <c r="H32" s="1">
-        <v>3.84</v>
+        <v>5.15</v>
       </c>
       <c r="I32" s="1">
-        <v>3.63</v>
+        <v>4.93</v>
       </c>
       <c r="J32" s="1">
-        <v>3.96</v>
+        <v>4.28</v>
       </c>
       <c r="K32" s="1">
-        <v>3.49</v>
+        <v>4.18</v>
       </c>
       <c r="L32" s="1">
-        <v>3.98</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -1162,37 +1162,37 @@
         <v>20</v>
       </c>
       <c r="B35" s="1">
-        <v>14.49</v>
+        <v>15.8</v>
       </c>
       <c r="C35" s="1">
-        <v>14.77</v>
+        <v>16.02</v>
       </c>
       <c r="D35" s="1">
-        <v>15.18</v>
+        <v>15.97</v>
       </c>
       <c r="E35" s="1">
-        <v>15.28</v>
+        <v>15.49</v>
       </c>
       <c r="F35" s="1">
-        <v>15.21</v>
+        <v>16.13</v>
       </c>
       <c r="G35" s="1">
-        <v>15.55</v>
+        <v>16.14</v>
       </c>
       <c r="H35" s="1">
-        <v>15.62</v>
+        <v>15.9</v>
       </c>
       <c r="I35" s="1">
-        <v>15.58</v>
+        <v>15.92</v>
       </c>
       <c r="J35" s="1">
-        <v>15.68</v>
+        <v>15.88</v>
       </c>
       <c r="K35" s="1">
-        <v>15.63</v>
+        <v>15.97</v>
       </c>
       <c r="L35" s="1">
-        <v>15.76</v>
+        <v>16.13</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -1200,37 +1200,37 @@
         <v>21</v>
       </c>
       <c r="B36" s="1">
-        <v>19.33</v>
+        <v>20.65</v>
       </c>
       <c r="C36" s="1">
-        <v>19.83</v>
+        <v>21.14</v>
       </c>
       <c r="D36" s="1">
-        <v>20.56</v>
+        <v>21.42</v>
       </c>
       <c r="E36" s="1">
-        <v>21.07</v>
+        <v>24.23</v>
       </c>
       <c r="F36" s="1">
-        <v>24.12</v>
+        <v>25.09</v>
       </c>
       <c r="G36" s="1">
-        <v>24.67</v>
+        <v>25.14</v>
       </c>
       <c r="H36" s="1">
-        <v>24.76</v>
+        <v>25</v>
       </c>
       <c r="I36" s="1">
-        <v>24.73</v>
+        <v>25.05</v>
       </c>
       <c r="J36" s="1">
-        <v>24.84</v>
+        <v>25.06</v>
       </c>
       <c r="K36" s="1">
-        <v>24.81</v>
+        <v>25.19</v>
       </c>
       <c r="L36" s="1">
-        <v>24.94</v>
+        <v>25.38</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -1238,37 +1238,37 @@
         <v>22</v>
       </c>
       <c r="B37" s="1">
-        <v>27.4</v>
+        <v>27.97</v>
       </c>
       <c r="C37" s="1">
-        <v>27.34</v>
+        <v>27.97</v>
       </c>
       <c r="D37" s="1">
-        <v>27.48</v>
+        <v>27.69</v>
       </c>
       <c r="E37" s="1">
-        <v>27.43</v>
+        <v>31.07</v>
       </c>
       <c r="F37" s="1">
-        <v>30.96</v>
+        <v>31.2</v>
       </c>
       <c r="G37" s="1">
-        <v>30.94</v>
+        <v>31.23</v>
       </c>
       <c r="H37" s="1">
-        <v>31.01</v>
+        <v>31.09</v>
       </c>
       <c r="I37" s="1">
-        <v>30.98</v>
+        <v>31.15</v>
       </c>
       <c r="J37" s="1">
-        <v>31.08</v>
+        <v>31.16</v>
       </c>
       <c r="K37" s="1">
-        <v>31.06</v>
+        <v>31.3</v>
       </c>
       <c r="L37" s="1">
-        <v>31.17</v>
+        <v>31.48</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -1276,37 +1276,37 @@
         <v>23</v>
       </c>
       <c r="B38" s="1">
-        <v>6.71</v>
+        <v>7.98</v>
       </c>
       <c r="C38" s="1">
-        <v>6.58</v>
+        <v>7.65</v>
       </c>
       <c r="D38" s="1">
-        <v>6.35</v>
+        <v>6.99</v>
       </c>
       <c r="E38" s="1">
-        <v>5.66</v>
+        <v>-0.71</v>
       </c>
       <c r="F38" s="1">
-        <v>-1.42</v>
+        <v>-0.68</v>
       </c>
       <c r="G38" s="1">
-        <v>-1.61</v>
+        <v>-0.77</v>
       </c>
       <c r="H38" s="1">
-        <v>-1.6</v>
+        <v>-1.21</v>
       </c>
       <c r="I38" s="1">
-        <v>-1.65</v>
+        <v>-1.26</v>
       </c>
       <c r="J38" s="1">
-        <v>-1.58</v>
+        <v>-1.43</v>
       </c>
       <c r="K38" s="1">
-        <v>-1.68</v>
+        <v>-1.46</v>
       </c>
       <c r="L38" s="1">
-        <v>-1.58</v>
+        <v>-1.39</v>
       </c>
     </row>
     <row r="40" spans="1:12">

</xml_diff>

<commit_message>
Update data and code for February 2024 baseline
</commit_message>
<xml_diff>
--- a/captax/data/outputs/Current-Law/comprehensive/supplemental_table_EMTRs_Current-Law_comprehensive.xlsx
+++ b/captax/data/outputs/Current-Law/comprehensive/supplemental_table_EMTRs_Current-Law_comprehensive.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>Effective Marginal Tax Rates on Capital Income, by Tax Year</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Data source: Congressional Budget Office.</t>
+  </si>
+  <si>
+    <t>* = between zero and 0.05 percentage points.</t>
   </si>
 </sst>
 </file>
@@ -184,7 +187,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="166" formatCode="&quot;*&quot;;&quot;*&quot;"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -510,37 +517,37 @@
     </row>
     <row r="9" spans="1:12">
       <c r="B9" s="5">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C9" s="5">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="D9" s="5">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="E9" s="5">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="F9" s="5">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="G9" s="5">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="H9" s="5">
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="I9" s="5">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="J9" s="5">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="K9" s="5">
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="L9" s="5">
-        <v>2033</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -567,37 +574,37 @@
         <v>3</v>
       </c>
       <c r="B12" s="1">
-        <v>15.28</v>
+        <v>14.23</v>
       </c>
       <c r="C12" s="1">
-        <v>15.63</v>
+        <v>14.56</v>
       </c>
       <c r="D12" s="1">
-        <v>15.74</v>
+        <v>14.7</v>
       </c>
       <c r="E12" s="1">
-        <v>15.62</v>
+        <v>15.51</v>
       </c>
       <c r="F12" s="1">
-        <v>16.44</v>
+        <v>15.47</v>
       </c>
       <c r="G12" s="1">
-        <v>16.46</v>
+        <v>15.27</v>
       </c>
       <c r="H12" s="1">
-        <v>16.24</v>
+        <v>15.38</v>
       </c>
       <c r="I12" s="1">
-        <v>16.26</v>
+        <v>15.39</v>
       </c>
       <c r="J12" s="1">
-        <v>16.23</v>
+        <v>15.47</v>
       </c>
       <c r="K12" s="1">
-        <v>16.32</v>
+        <v>15.5</v>
       </c>
       <c r="L12" s="1">
-        <v>16.49</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -605,37 +612,37 @@
         <v>4</v>
       </c>
       <c r="B14" s="1">
-        <v>18.84</v>
+        <v>18.16</v>
       </c>
       <c r="C14" s="1">
-        <v>19.47</v>
+        <v>18.96</v>
       </c>
       <c r="D14" s="1">
-        <v>19.9</v>
+        <v>21.51</v>
       </c>
       <c r="E14" s="1">
-        <v>22.55</v>
+        <v>22.56</v>
       </c>
       <c r="F14" s="1">
-        <v>23.6</v>
+        <v>22.53</v>
       </c>
       <c r="G14" s="1">
-        <v>23.66</v>
+        <v>22.45</v>
       </c>
       <c r="H14" s="1">
-        <v>23.52</v>
+        <v>22.65</v>
       </c>
       <c r="I14" s="1">
-        <v>23.56</v>
+        <v>22.66</v>
       </c>
       <c r="J14" s="1">
-        <v>23.58</v>
+        <v>22.73</v>
       </c>
       <c r="K14" s="1">
-        <v>23.71</v>
+        <v>22.79</v>
       </c>
       <c r="L14" s="1">
-        <v>23.9</v>
+        <v>22.72</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -648,37 +655,37 @@
         <v>6</v>
       </c>
       <c r="B16" s="1">
-        <v>9.84</v>
+        <v>10.54</v>
       </c>
       <c r="C16" s="1">
-        <v>12.12</v>
+        <v>12.82</v>
       </c>
       <c r="D16" s="1">
-        <v>14.27</v>
+        <v>15.76</v>
       </c>
       <c r="E16" s="1">
-        <v>17.2</v>
+        <v>18.76</v>
       </c>
       <c r="F16" s="1">
-        <v>20.28</v>
+        <v>18.81</v>
       </c>
       <c r="G16" s="1">
-        <v>20.35</v>
+        <v>18.83</v>
       </c>
       <c r="H16" s="1">
-        <v>20.21</v>
+        <v>19.17</v>
       </c>
       <c r="I16" s="1">
-        <v>20.25</v>
+        <v>19.19</v>
       </c>
       <c r="J16" s="1">
-        <v>20.27</v>
+        <v>19.32</v>
       </c>
       <c r="K16" s="1">
-        <v>20.38</v>
+        <v>19.36</v>
       </c>
       <c r="L16" s="1">
-        <v>20.57</v>
+        <v>19.31</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -686,37 +693,37 @@
         <v>7</v>
       </c>
       <c r="B17" s="1">
-        <v>21.02</v>
+        <v>19.87</v>
       </c>
       <c r="C17" s="1">
-        <v>21.27</v>
+        <v>20.33</v>
       </c>
       <c r="D17" s="1">
-        <v>21.27</v>
+        <v>22.29</v>
       </c>
       <c r="E17" s="1">
-        <v>23.22</v>
+        <v>23.04</v>
       </c>
       <c r="F17" s="1">
-        <v>23.88</v>
+        <v>22.96</v>
       </c>
       <c r="G17" s="1">
-        <v>23.94</v>
+        <v>22.8</v>
       </c>
       <c r="H17" s="1">
-        <v>23.81</v>
+        <v>22.9</v>
       </c>
       <c r="I17" s="1">
-        <v>23.85</v>
+        <v>22.89</v>
       </c>
       <c r="J17" s="1">
-        <v>23.87</v>
+        <v>22.94</v>
       </c>
       <c r="K17" s="1">
-        <v>23.99</v>
+        <v>23.01</v>
       </c>
       <c r="L17" s="1">
-        <v>24.18</v>
+        <v>22.94</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -724,37 +731,37 @@
         <v>8</v>
       </c>
       <c r="B18" s="1">
-        <v>25.29</v>
+        <v>24.22</v>
       </c>
       <c r="C18" s="1">
-        <v>25.38</v>
+        <v>24.49</v>
       </c>
       <c r="D18" s="1">
-        <v>25.09</v>
+        <v>28.36</v>
       </c>
       <c r="E18" s="1">
-        <v>29.2</v>
+        <v>28.51</v>
       </c>
       <c r="F18" s="1">
-        <v>29.39</v>
+        <v>28.44</v>
       </c>
       <c r="G18" s="1">
-        <v>29.41</v>
+        <v>28.24</v>
       </c>
       <c r="H18" s="1">
-        <v>29.25</v>
+        <v>28.24</v>
       </c>
       <c r="I18" s="1">
-        <v>29.31</v>
+        <v>28.28</v>
       </c>
       <c r="J18" s="1">
-        <v>29.31</v>
+        <v>28.3</v>
       </c>
       <c r="K18" s="1">
-        <v>29.46</v>
+        <v>28.35</v>
       </c>
       <c r="L18" s="1">
-        <v>29.64</v>
+        <v>28.27</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -762,37 +769,37 @@
         <v>9</v>
       </c>
       <c r="B19" s="1">
-        <v>-4.93</v>
+        <v>-7.62</v>
       </c>
       <c r="C19" s="1">
-        <v>-5.16</v>
+        <v>-7.34</v>
       </c>
       <c r="D19" s="1">
-        <v>-5.39</v>
+        <v>-5.86</v>
       </c>
       <c r="E19" s="1">
-        <v>-4.14</v>
+        <v>-5.32</v>
       </c>
       <c r="F19" s="1">
-        <v>-4.09</v>
+        <v>-4.87</v>
       </c>
       <c r="G19" s="1">
-        <v>-3.98</v>
+        <v>-3.89</v>
       </c>
       <c r="H19" s="1">
-        <v>-4.14</v>
+        <v>-2.17</v>
       </c>
       <c r="I19" s="1">
-        <v>-4.06</v>
+        <v>-2.06</v>
       </c>
       <c r="J19" s="1">
-        <v>-3.98</v>
+        <v>-1.86</v>
       </c>
       <c r="K19" s="1">
-        <v>-3.78</v>
+        <v>-1.82</v>
       </c>
       <c r="L19" s="1">
-        <v>-3.5</v>
+        <v>-1.85</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -800,37 +807,37 @@
         <v>10</v>
       </c>
       <c r="B20" s="1">
-        <v>14.52</v>
+        <v>17.58</v>
       </c>
       <c r="C20" s="1">
-        <v>18.13</v>
+        <v>21.04</v>
       </c>
       <c r="D20" s="1">
-        <v>21.45</v>
+        <v>24.84</v>
       </c>
       <c r="E20" s="1">
-        <v>25.17</v>
+        <v>27.92</v>
       </c>
       <c r="F20" s="1">
-        <v>28.21</v>
+        <v>27.93</v>
       </c>
       <c r="G20" s="1">
-        <v>28.28</v>
+        <v>27.84</v>
       </c>
       <c r="H20" s="1">
-        <v>28.15</v>
+        <v>28.01</v>
       </c>
       <c r="I20" s="1">
-        <v>28.18</v>
+        <v>28.01</v>
       </c>
       <c r="J20" s="1">
-        <v>28.2</v>
+        <v>28.13</v>
       </c>
       <c r="K20" s="1">
-        <v>28.31</v>
+        <v>28.17</v>
       </c>
       <c r="L20" s="1">
-        <v>28.5</v>
+        <v>28.14</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -838,37 +845,37 @@
         <v>11</v>
       </c>
       <c r="B21" s="1">
-        <v>30.6</v>
+        <v>29.82</v>
       </c>
       <c r="C21" s="1">
-        <v>30.54</v>
+        <v>29.94</v>
       </c>
       <c r="D21" s="1">
-        <v>30.33</v>
+        <v>32.28</v>
       </c>
       <c r="E21" s="1">
-        <v>33.15</v>
+        <v>32.36</v>
       </c>
       <c r="F21" s="1">
-        <v>33.26</v>
+        <v>32.3</v>
       </c>
       <c r="G21" s="1">
-        <v>33.31</v>
+        <v>32.15</v>
       </c>
       <c r="H21" s="1">
-        <v>33.2</v>
+        <v>32.18</v>
       </c>
       <c r="I21" s="1">
-        <v>33.24</v>
+        <v>32.19</v>
       </c>
       <c r="J21" s="1">
-        <v>33.26</v>
+        <v>32.25</v>
       </c>
       <c r="K21" s="1">
-        <v>33.39</v>
+        <v>32.29</v>
       </c>
       <c r="L21" s="1">
-        <v>33.55</v>
+        <v>32.24</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -881,37 +888,37 @@
         <v>13</v>
       </c>
       <c r="B23" s="1">
-        <v>20.94</v>
+        <v>20.89</v>
       </c>
       <c r="C23" s="1">
-        <v>21.57</v>
+        <v>21.7</v>
       </c>
       <c r="D23" s="1">
-        <v>22.07</v>
+        <v>24.52</v>
       </c>
       <c r="E23" s="1">
-        <v>25.16</v>
+        <v>25.45</v>
       </c>
       <c r="F23" s="1">
-        <v>26.15</v>
+        <v>25.4</v>
       </c>
       <c r="G23" s="1">
-        <v>26.21</v>
+        <v>25.42</v>
       </c>
       <c r="H23" s="1">
-        <v>26.14</v>
+        <v>25.62</v>
       </c>
       <c r="I23" s="1">
-        <v>26.15</v>
+        <v>25.63</v>
       </c>
       <c r="J23" s="1">
-        <v>26.17</v>
+        <v>25.65</v>
       </c>
       <c r="K23" s="1">
-        <v>26.27</v>
+        <v>25.71</v>
       </c>
       <c r="L23" s="1">
-        <v>26.37</v>
+        <v>25.68</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -919,37 +926,37 @@
         <v>14</v>
       </c>
       <c r="B24" s="1">
-        <v>9.59</v>
+        <v>6.07</v>
       </c>
       <c r="C24" s="1">
-        <v>10.26</v>
+        <v>6.72</v>
       </c>
       <c r="D24" s="1">
-        <v>10.34</v>
+        <v>7.39</v>
       </c>
       <c r="E24" s="1">
-        <v>10.29</v>
+        <v>9.09</v>
       </c>
       <c r="F24" s="1">
-        <v>11.57</v>
+        <v>9.15</v>
       </c>
       <c r="G24" s="1">
-        <v>11.63</v>
+        <v>8.640000000000001</v>
       </c>
       <c r="H24" s="1">
-        <v>11.19</v>
+        <v>8.83</v>
       </c>
       <c r="I24" s="1">
-        <v>11.41</v>
+        <v>8.85</v>
       </c>
       <c r="J24" s="1">
-        <v>11.44</v>
+        <v>9.140000000000001</v>
       </c>
       <c r="K24" s="1">
-        <v>11.74</v>
+        <v>9.19</v>
       </c>
       <c r="L24" s="1">
-        <v>12.37</v>
+        <v>8.960000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -962,37 +969,37 @@
         <v>16</v>
       </c>
       <c r="B26" s="1">
-        <v>17.58</v>
+        <v>17.03</v>
       </c>
       <c r="C26" s="1">
-        <v>18.2</v>
+        <v>17.79</v>
       </c>
       <c r="D26" s="1">
-        <v>18.76</v>
+        <v>19.06</v>
       </c>
       <c r="E26" s="1">
-        <v>19.88</v>
+        <v>20.23</v>
       </c>
       <c r="F26" s="1">
-        <v>21.04</v>
+        <v>20.23</v>
       </c>
       <c r="G26" s="1">
-        <v>21.13</v>
+        <v>20.21</v>
       </c>
       <c r="H26" s="1">
-        <v>21</v>
+        <v>20.49</v>
       </c>
       <c r="I26" s="1">
-        <v>21.03</v>
+        <v>20.48</v>
       </c>
       <c r="J26" s="1">
-        <v>21.06</v>
+        <v>20.58</v>
       </c>
       <c r="K26" s="1">
-        <v>21.17</v>
+        <v>20.64</v>
       </c>
       <c r="L26" s="1">
-        <v>21.36</v>
+        <v>20.6</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1000,37 +1007,37 @@
         <v>17</v>
       </c>
       <c r="B27" s="1">
-        <v>21.66</v>
+        <v>20.99</v>
       </c>
       <c r="C27" s="1">
-        <v>22.33</v>
+        <v>21.86</v>
       </c>
       <c r="D27" s="1">
-        <v>22.48</v>
+        <v>27.28</v>
       </c>
       <c r="E27" s="1">
-        <v>28.2</v>
+        <v>28.08</v>
       </c>
       <c r="F27" s="1">
-        <v>29.04</v>
+        <v>27.99</v>
       </c>
       <c r="G27" s="1">
-        <v>29.04</v>
+        <v>27.79</v>
       </c>
       <c r="H27" s="1">
-        <v>28.88</v>
+        <v>27.79</v>
       </c>
       <c r="I27" s="1">
-        <v>28.95</v>
+        <v>27.85</v>
       </c>
       <c r="J27" s="1">
-        <v>28.95</v>
+        <v>27.84</v>
       </c>
       <c r="K27" s="1">
-        <v>29.11</v>
+        <v>27.89</v>
       </c>
       <c r="L27" s="1">
-        <v>29.29</v>
+        <v>27.79</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1038,37 +1045,37 @@
         <v>18</v>
       </c>
       <c r="B29" s="1">
-        <v>7.98</v>
+        <v>6.91</v>
       </c>
       <c r="C29" s="1">
-        <v>7.65</v>
+        <v>6.21</v>
       </c>
       <c r="D29" s="1">
-        <v>6.99</v>
+        <v>0.5</v>
       </c>
       <c r="E29" s="1">
-        <v>-0.71</v>
+        <v>0.59</v>
       </c>
       <c r="F29" s="1">
-        <v>-0.68</v>
+        <v>0.54</v>
       </c>
       <c r="G29" s="1">
-        <v>-0.77</v>
+        <v>0.04</v>
       </c>
       <c r="H29" s="1">
-        <v>-1.21</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="I29" s="1">
-        <v>-1.26</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="J29" s="1">
-        <v>-1.43</v>
+        <v>0.04</v>
       </c>
       <c r="K29" s="1">
-        <v>-1.46</v>
+        <v>0</v>
       </c>
       <c r="L29" s="1">
-        <v>-1.39</v>
+        <v>-0.19</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1081,37 +1088,37 @@
         <v>13</v>
       </c>
       <c r="B31" s="1">
-        <v>-0.23</v>
+        <v>-0.18</v>
       </c>
       <c r="C31" s="1">
-        <v>-0.23</v>
+        <v>-0.2</v>
       </c>
       <c r="D31" s="1">
-        <v>-0.24</v>
+        <v>-2.31</v>
       </c>
       <c r="E31" s="1">
-        <v>-3.32</v>
+        <v>-2.34</v>
       </c>
       <c r="F31" s="1">
-        <v>-3.38</v>
+        <v>-2.34</v>
       </c>
       <c r="G31" s="1">
-        <v>-3.38</v>
+        <v>-2.33</v>
       </c>
       <c r="H31" s="1">
-        <v>-3.37</v>
+        <v>-2.33</v>
       </c>
       <c r="I31" s="1">
-        <v>-3.37</v>
+        <v>-2.32</v>
       </c>
       <c r="J31" s="1">
-        <v>-3.37</v>
+        <v>-2.32</v>
       </c>
       <c r="K31" s="1">
-        <v>-3.37</v>
+        <v>-2.32</v>
       </c>
       <c r="L31" s="1">
-        <v>-3.37</v>
+        <v>-2.32</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -1119,37 +1126,37 @@
         <v>14</v>
       </c>
       <c r="B32" s="1">
-        <v>26.85</v>
+        <v>22.91</v>
       </c>
       <c r="C32" s="1">
-        <v>26.01</v>
+        <v>21.04</v>
       </c>
       <c r="D32" s="1">
-        <v>24.12</v>
+        <v>8.140000000000001</v>
       </c>
       <c r="E32" s="1">
-        <v>6.87</v>
+        <v>8.539999999999999</v>
       </c>
       <c r="F32" s="1">
-        <v>7.19</v>
+        <v>8.369999999999999</v>
       </c>
       <c r="G32" s="1">
-        <v>6.85</v>
+        <v>6.53</v>
       </c>
       <c r="H32" s="1">
-        <v>5.15</v>
+        <v>6.12</v>
       </c>
       <c r="I32" s="1">
-        <v>4.93</v>
+        <v>6.09</v>
       </c>
       <c r="J32" s="1">
-        <v>4.28</v>
+        <v>6.51</v>
       </c>
       <c r="K32" s="1">
-        <v>4.18</v>
+        <v>6.38</v>
       </c>
       <c r="L32" s="1">
-        <v>4.5</v>
+        <v>5.65</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -1162,37 +1169,37 @@
         <v>20</v>
       </c>
       <c r="B35" s="1">
-        <v>15.8</v>
+        <v>14.82</v>
       </c>
       <c r="C35" s="1">
-        <v>16.02</v>
+        <v>14.99</v>
       </c>
       <c r="D35" s="1">
-        <v>15.97</v>
+        <v>14.88</v>
       </c>
       <c r="E35" s="1">
         <v>15.49</v>
       </c>
       <c r="F35" s="1">
-        <v>16.13</v>
+        <v>15.45</v>
       </c>
       <c r="G35" s="1">
-        <v>16.14</v>
+        <v>15.21</v>
       </c>
       <c r="H35" s="1">
-        <v>15.9</v>
+        <v>15.28</v>
       </c>
       <c r="I35" s="1">
-        <v>15.92</v>
+        <v>15.29</v>
       </c>
       <c r="J35" s="1">
-        <v>15.88</v>
+        <v>15.37</v>
       </c>
       <c r="K35" s="1">
-        <v>15.97</v>
+        <v>15.4</v>
       </c>
       <c r="L35" s="1">
-        <v>16.13</v>
+        <v>15.28</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -1200,37 +1207,37 @@
         <v>21</v>
       </c>
       <c r="B36" s="1">
-        <v>20.65</v>
+        <v>20.18</v>
       </c>
       <c r="C36" s="1">
-        <v>21.14</v>
+        <v>20.83</v>
       </c>
       <c r="D36" s="1">
-        <v>21.42</v>
+        <v>23.57</v>
       </c>
       <c r="E36" s="1">
-        <v>24.23</v>
+        <v>24.4</v>
       </c>
       <c r="F36" s="1">
-        <v>25.09</v>
+        <v>24.36</v>
       </c>
       <c r="G36" s="1">
-        <v>25.14</v>
+        <v>24.26</v>
       </c>
       <c r="H36" s="1">
-        <v>25</v>
+        <v>24.41</v>
       </c>
       <c r="I36" s="1">
-        <v>25.05</v>
+        <v>24.43</v>
       </c>
       <c r="J36" s="1">
-        <v>25.06</v>
+        <v>24.49</v>
       </c>
       <c r="K36" s="1">
-        <v>25.19</v>
+        <v>24.55</v>
       </c>
       <c r="L36" s="1">
-        <v>25.38</v>
+        <v>24.48</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -1238,37 +1245,37 @@
         <v>22</v>
       </c>
       <c r="B37" s="1">
-        <v>27.97</v>
+        <v>27.4</v>
       </c>
       <c r="C37" s="1">
-        <v>27.97</v>
+        <v>27.6</v>
       </c>
       <c r="D37" s="1">
-        <v>27.69</v>
+        <v>30.93</v>
       </c>
       <c r="E37" s="1">
-        <v>31.07</v>
+        <v>31.03</v>
       </c>
       <c r="F37" s="1">
-        <v>31.2</v>
+        <v>30.96</v>
       </c>
       <c r="G37" s="1">
-        <v>31.23</v>
+        <v>30.78</v>
       </c>
       <c r="H37" s="1">
-        <v>31.09</v>
+        <v>30.79</v>
       </c>
       <c r="I37" s="1">
-        <v>31.15</v>
+        <v>30.82</v>
       </c>
       <c r="J37" s="1">
-        <v>31.16</v>
+        <v>30.86</v>
       </c>
       <c r="K37" s="1">
-        <v>31.3</v>
+        <v>30.91</v>
       </c>
       <c r="L37" s="1">
-        <v>31.48</v>
+        <v>30.84</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -1276,37 +1283,37 @@
         <v>23</v>
       </c>
       <c r="B38" s="1">
-        <v>7.98</v>
+        <v>6.91</v>
       </c>
       <c r="C38" s="1">
-        <v>7.65</v>
+        <v>6.21</v>
       </c>
       <c r="D38" s="1">
-        <v>6.99</v>
+        <v>0.5</v>
       </c>
       <c r="E38" s="1">
-        <v>-0.71</v>
+        <v>0.59</v>
       </c>
       <c r="F38" s="1">
-        <v>-0.68</v>
+        <v>0.54</v>
       </c>
       <c r="G38" s="1">
-        <v>-0.77</v>
+        <v>0.04</v>
       </c>
       <c r="H38" s="1">
-        <v>-1.21</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="I38" s="1">
-        <v>-1.26</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="J38" s="1">
-        <v>-1.43</v>
+        <v>0.04</v>
       </c>
       <c r="K38" s="1">
-        <v>-1.46</v>
+        <v>0</v>
       </c>
       <c r="L38" s="1">
-        <v>-1.39</v>
+        <v>-0.19</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -1328,6 +1335,11 @@
         <v>24</v>
       </c>
     </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="45" spans="1:12">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
@@ -1343,6 +1355,12 @@
       <c r="L45" s="4"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B12:L38">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
+      <formula>0.001</formula>
+      <formula>0.049</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update data for June 2024 baseline
</commit_message>
<xml_diff>
--- a/captax/data/outputs/Current-Law/comprehensive/supplemental_table_EMTRs_Current-Law_comprehensive.xlsx
+++ b/captax/data/outputs/Current-Law/comprehensive/supplemental_table_EMTRs_Current-Law_comprehensive.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Effective Marginal Tax Rates on Capital Income, by Tax Year</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>Data source: Congressional Budget Office.</t>
-  </si>
-  <si>
-    <t>* = between zero and 0.05 percentage points.</t>
   </si>
 </sst>
 </file>
@@ -187,11 +184,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <numFmt numFmtId="166" formatCode="&quot;*&quot;;&quot;*&quot;"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -574,37 +567,37 @@
         <v>3</v>
       </c>
       <c r="B12" s="1">
-        <v>14.23</v>
+        <v>14.46</v>
       </c>
       <c r="C12" s="1">
-        <v>14.56</v>
+        <v>14.86</v>
       </c>
       <c r="D12" s="1">
-        <v>14.7</v>
+        <v>14.49</v>
       </c>
       <c r="E12" s="1">
-        <v>15.51</v>
+        <v>15.07</v>
       </c>
       <c r="F12" s="1">
-        <v>15.47</v>
+        <v>15.09</v>
       </c>
       <c r="G12" s="1">
-        <v>15.27</v>
+        <v>15.05</v>
       </c>
       <c r="H12" s="1">
-        <v>15.38</v>
+        <v>15.15</v>
       </c>
       <c r="I12" s="1">
-        <v>15.39</v>
+        <v>15.19</v>
       </c>
       <c r="J12" s="1">
-        <v>15.47</v>
+        <v>15.24</v>
       </c>
       <c r="K12" s="1">
-        <v>15.5</v>
+        <v>15.25</v>
       </c>
       <c r="L12" s="1">
-        <v>15.4</v>
+        <v>15.29</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -612,37 +605,37 @@
         <v>4</v>
       </c>
       <c r="B14" s="1">
-        <v>18.16</v>
+        <v>17.82</v>
       </c>
       <c r="C14" s="1">
-        <v>18.96</v>
+        <v>18.53</v>
       </c>
       <c r="D14" s="1">
-        <v>21.51</v>
+        <v>21.03</v>
       </c>
       <c r="E14" s="1">
-        <v>22.56</v>
+        <v>21.93</v>
       </c>
       <c r="F14" s="1">
-        <v>22.53</v>
+        <v>21.96</v>
       </c>
       <c r="G14" s="1">
-        <v>22.45</v>
+        <v>21.98</v>
       </c>
       <c r="H14" s="1">
-        <v>22.65</v>
+        <v>22.17</v>
       </c>
       <c r="I14" s="1">
-        <v>22.66</v>
+        <v>22.21</v>
       </c>
       <c r="J14" s="1">
-        <v>22.73</v>
+        <v>22.25</v>
       </c>
       <c r="K14" s="1">
-        <v>22.79</v>
+        <v>22.27</v>
       </c>
       <c r="L14" s="1">
-        <v>22.72</v>
+        <v>22.32</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -655,37 +648,37 @@
         <v>6</v>
       </c>
       <c r="B16" s="1">
-        <v>10.54</v>
+        <v>10.21</v>
       </c>
       <c r="C16" s="1">
-        <v>12.82</v>
+        <v>12.49</v>
       </c>
       <c r="D16" s="1">
-        <v>15.76</v>
+        <v>15.31</v>
       </c>
       <c r="E16" s="1">
-        <v>18.76</v>
+        <v>18.13</v>
       </c>
       <c r="F16" s="1">
+        <v>18.25</v>
+      </c>
+      <c r="G16" s="1">
+        <v>18.37</v>
+      </c>
+      <c r="H16" s="1">
+        <v>18.74</v>
+      </c>
+      <c r="I16" s="1">
         <v>18.81</v>
       </c>
-      <c r="G16" s="1">
-        <v>18.83</v>
-      </c>
-      <c r="H16" s="1">
-        <v>19.17</v>
-      </c>
-      <c r="I16" s="1">
-        <v>19.19</v>
-      </c>
       <c r="J16" s="1">
-        <v>19.32</v>
+        <v>18.88</v>
       </c>
       <c r="K16" s="1">
-        <v>19.36</v>
+        <v>18.89</v>
       </c>
       <c r="L16" s="1">
-        <v>19.31</v>
+        <v>18.96</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -693,37 +686,37 @@
         <v>7</v>
       </c>
       <c r="B17" s="1">
-        <v>19.87</v>
+        <v>19.51</v>
       </c>
       <c r="C17" s="1">
-        <v>20.33</v>
+        <v>19.9</v>
       </c>
       <c r="D17" s="1">
-        <v>22.29</v>
+        <v>21.81</v>
       </c>
       <c r="E17" s="1">
-        <v>23.04</v>
+        <v>22.4</v>
       </c>
       <c r="F17" s="1">
-        <v>22.96</v>
+        <v>22.37</v>
       </c>
       <c r="G17" s="1">
-        <v>22.8</v>
+        <v>22.32</v>
       </c>
       <c r="H17" s="1">
-        <v>22.9</v>
+        <v>22.43</v>
       </c>
       <c r="I17" s="1">
-        <v>22.89</v>
+        <v>22.45</v>
       </c>
       <c r="J17" s="1">
-        <v>22.94</v>
+        <v>22.45</v>
       </c>
       <c r="K17" s="1">
-        <v>23.01</v>
+        <v>22.5</v>
       </c>
       <c r="L17" s="1">
-        <v>22.94</v>
+        <v>22.53</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -731,37 +724,37 @@
         <v>8</v>
       </c>
       <c r="B18" s="1">
-        <v>24.22</v>
+        <v>23.96</v>
       </c>
       <c r="C18" s="1">
-        <v>24.49</v>
+        <v>24.01</v>
       </c>
       <c r="D18" s="1">
-        <v>28.36</v>
+        <v>27.88</v>
       </c>
       <c r="E18" s="1">
-        <v>28.51</v>
+        <v>27.91</v>
       </c>
       <c r="F18" s="1">
-        <v>28.44</v>
+        <v>27.86</v>
       </c>
       <c r="G18" s="1">
-        <v>28.24</v>
+        <v>27.78</v>
       </c>
       <c r="H18" s="1">
-        <v>28.24</v>
+        <v>27.74</v>
       </c>
       <c r="I18" s="1">
-        <v>28.28</v>
+        <v>27.74</v>
       </c>
       <c r="J18" s="1">
-        <v>28.3</v>
+        <v>27.78</v>
       </c>
       <c r="K18" s="1">
-        <v>28.35</v>
+        <v>27.79</v>
       </c>
       <c r="L18" s="1">
-        <v>28.27</v>
+        <v>27.82</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -769,37 +762,37 @@
         <v>9</v>
       </c>
       <c r="B19" s="1">
-        <v>-7.62</v>
+        <v>-7.97</v>
       </c>
       <c r="C19" s="1">
-        <v>-7.34</v>
+        <v>-7.72</v>
       </c>
       <c r="D19" s="1">
-        <v>-5.86</v>
+        <v>-6.37</v>
       </c>
       <c r="E19" s="1">
-        <v>-5.32</v>
+        <v>-6.06</v>
       </c>
       <c r="F19" s="1">
-        <v>-4.87</v>
+        <v>-5.54</v>
       </c>
       <c r="G19" s="1">
-        <v>-3.89</v>
+        <v>-4.47</v>
       </c>
       <c r="H19" s="1">
-        <v>-2.17</v>
+        <v>-2.71</v>
       </c>
       <c r="I19" s="1">
-        <v>-2.06</v>
+        <v>-2.52</v>
       </c>
       <c r="J19" s="1">
-        <v>-1.86</v>
+        <v>-2.41</v>
       </c>
       <c r="K19" s="1">
-        <v>-1.82</v>
+        <v>-2.4</v>
       </c>
       <c r="L19" s="1">
-        <v>-1.85</v>
+        <v>-2.31</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -807,37 +800,37 @@
         <v>10</v>
       </c>
       <c r="B20" s="1">
-        <v>17.58</v>
+        <v>17.19</v>
       </c>
       <c r="C20" s="1">
-        <v>21.04</v>
+        <v>20.66</v>
       </c>
       <c r="D20" s="1">
-        <v>24.84</v>
+        <v>24.39</v>
       </c>
       <c r="E20" s="1">
-        <v>27.92</v>
+        <v>27.34</v>
       </c>
       <c r="F20" s="1">
-        <v>27.93</v>
+        <v>27.4</v>
       </c>
       <c r="G20" s="1">
-        <v>27.84</v>
+        <v>27.4</v>
       </c>
       <c r="H20" s="1">
-        <v>28.01</v>
+        <v>27.59</v>
       </c>
       <c r="I20" s="1">
-        <v>28.01</v>
+        <v>27.65</v>
       </c>
       <c r="J20" s="1">
-        <v>28.13</v>
+        <v>27.71</v>
       </c>
       <c r="K20" s="1">
-        <v>28.17</v>
+        <v>27.73</v>
       </c>
       <c r="L20" s="1">
-        <v>28.14</v>
+        <v>27.79</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -845,37 +838,37 @@
         <v>11</v>
       </c>
       <c r="B21" s="1">
-        <v>29.82</v>
+        <v>29.5</v>
       </c>
       <c r="C21" s="1">
-        <v>29.94</v>
+        <v>29.48</v>
       </c>
       <c r="D21" s="1">
-        <v>32.28</v>
+        <v>31.82</v>
       </c>
       <c r="E21" s="1">
-        <v>32.36</v>
+        <v>31.79</v>
       </c>
       <c r="F21" s="1">
-        <v>32.3</v>
+        <v>31.77</v>
       </c>
       <c r="G21" s="1">
-        <v>32.15</v>
+        <v>31.69</v>
       </c>
       <c r="H21" s="1">
-        <v>32.18</v>
+        <v>31.71</v>
       </c>
       <c r="I21" s="1">
-        <v>32.19</v>
+        <v>31.73</v>
       </c>
       <c r="J21" s="1">
-        <v>32.25</v>
+        <v>31.78</v>
       </c>
       <c r="K21" s="1">
-        <v>32.29</v>
+        <v>31.79</v>
       </c>
       <c r="L21" s="1">
-        <v>32.24</v>
+        <v>31.83</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -888,37 +881,37 @@
         <v>13</v>
       </c>
       <c r="B23" s="1">
-        <v>20.89</v>
+        <v>20.54</v>
       </c>
       <c r="C23" s="1">
-        <v>21.7</v>
+        <v>21.25</v>
       </c>
       <c r="D23" s="1">
-        <v>24.52</v>
+        <v>24.11</v>
       </c>
       <c r="E23" s="1">
-        <v>25.45</v>
+        <v>24.98</v>
       </c>
       <c r="F23" s="1">
-        <v>25.4</v>
+        <v>24.96</v>
       </c>
       <c r="G23" s="1">
-        <v>25.42</v>
+        <v>24.99</v>
       </c>
       <c r="H23" s="1">
-        <v>25.62</v>
+        <v>25.18</v>
       </c>
       <c r="I23" s="1">
-        <v>25.63</v>
+        <v>25.19</v>
       </c>
       <c r="J23" s="1">
-        <v>25.65</v>
+        <v>25.21</v>
       </c>
       <c r="K23" s="1">
-        <v>25.71</v>
+        <v>25.24</v>
       </c>
       <c r="L23" s="1">
-        <v>25.68</v>
+        <v>25.26</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -926,37 +919,37 @@
         <v>14</v>
       </c>
       <c r="B24" s="1">
-        <v>6.07</v>
+        <v>5.45</v>
       </c>
       <c r="C24" s="1">
-        <v>6.72</v>
+        <v>6.15</v>
       </c>
       <c r="D24" s="1">
-        <v>7.39</v>
+        <v>6.15</v>
       </c>
       <c r="E24" s="1">
-        <v>9.09</v>
+        <v>7.27</v>
       </c>
       <c r="F24" s="1">
-        <v>9.15</v>
+        <v>7.53</v>
       </c>
       <c r="G24" s="1">
-        <v>8.640000000000001</v>
+        <v>7.46</v>
       </c>
       <c r="H24" s="1">
-        <v>8.83</v>
+        <v>7.74</v>
       </c>
       <c r="I24" s="1">
-        <v>8.85</v>
+        <v>7.91</v>
       </c>
       <c r="J24" s="1">
-        <v>9.140000000000001</v>
+        <v>8.02</v>
       </c>
       <c r="K24" s="1">
-        <v>9.19</v>
+        <v>8.02</v>
       </c>
       <c r="L24" s="1">
-        <v>8.960000000000001</v>
+        <v>8.18</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -969,37 +962,37 @@
         <v>16</v>
       </c>
       <c r="B26" s="1">
-        <v>17.03</v>
+        <v>16.63</v>
       </c>
       <c r="C26" s="1">
-        <v>17.79</v>
+        <v>17.39</v>
       </c>
       <c r="D26" s="1">
-        <v>19.06</v>
+        <v>18.58</v>
       </c>
       <c r="E26" s="1">
-        <v>20.23</v>
+        <v>19.59</v>
       </c>
       <c r="F26" s="1">
-        <v>20.23</v>
+        <v>19.66</v>
       </c>
       <c r="G26" s="1">
-        <v>20.21</v>
+        <v>19.72</v>
       </c>
       <c r="H26" s="1">
-        <v>20.49</v>
+        <v>20.04</v>
       </c>
       <c r="I26" s="1">
-        <v>20.48</v>
+        <v>20.1</v>
       </c>
       <c r="J26" s="1">
-        <v>20.58</v>
+        <v>20.13</v>
       </c>
       <c r="K26" s="1">
-        <v>20.64</v>
+        <v>20.17</v>
       </c>
       <c r="L26" s="1">
-        <v>20.6</v>
+        <v>20.22</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1007,37 +1000,37 @@
         <v>17</v>
       </c>
       <c r="B27" s="1">
-        <v>20.99</v>
+        <v>20.78</v>
       </c>
       <c r="C27" s="1">
-        <v>21.86</v>
+        <v>21.37</v>
       </c>
       <c r="D27" s="1">
-        <v>27.28</v>
+        <v>26.8</v>
       </c>
       <c r="E27" s="1">
-        <v>28.08</v>
+        <v>27.47</v>
       </c>
       <c r="F27" s="1">
-        <v>27.99</v>
+        <v>27.4</v>
       </c>
       <c r="G27" s="1">
-        <v>27.79</v>
+        <v>27.33</v>
       </c>
       <c r="H27" s="1">
-        <v>27.79</v>
+        <v>27.27</v>
       </c>
       <c r="I27" s="1">
-        <v>27.85</v>
+        <v>27.26</v>
       </c>
       <c r="J27" s="1">
-        <v>27.84</v>
+        <v>27.3</v>
       </c>
       <c r="K27" s="1">
-        <v>27.89</v>
+        <v>27.3</v>
       </c>
       <c r="L27" s="1">
-        <v>27.79</v>
+        <v>27.32</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1045,37 +1038,37 @@
         <v>18</v>
       </c>
       <c r="B29" s="1">
-        <v>6.91</v>
+        <v>8.279999999999999</v>
       </c>
       <c r="C29" s="1">
-        <v>6.21</v>
+        <v>8.039999999999999</v>
       </c>
       <c r="D29" s="1">
-        <v>0.5</v>
+        <v>0.96</v>
       </c>
       <c r="E29" s="1">
-        <v>0.59</v>
+        <v>0.68</v>
       </c>
       <c r="F29" s="1">
-        <v>0.54</v>
+        <v>0.67</v>
       </c>
       <c r="G29" s="1">
-        <v>0.04</v>
+        <v>0.51</v>
       </c>
       <c r="H29" s="1">
-        <v>-0.07000000000000001</v>
+        <v>0.37</v>
       </c>
       <c r="I29" s="1">
-        <v>-0.07000000000000001</v>
+        <v>0.4</v>
       </c>
       <c r="J29" s="1">
-        <v>0.04</v>
+        <v>0.48</v>
       </c>
       <c r="K29" s="1">
-        <v>0</v>
+        <v>0.43</v>
       </c>
       <c r="L29" s="1">
-        <v>-0.19</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1088,37 +1081,37 @@
         <v>13</v>
       </c>
       <c r="B31" s="1">
-        <v>-0.18</v>
+        <v>-0.15</v>
       </c>
       <c r="C31" s="1">
-        <v>-0.2</v>
+        <v>-0.15</v>
       </c>
       <c r="D31" s="1">
-        <v>-2.31</v>
+        <v>-2.23</v>
       </c>
       <c r="E31" s="1">
-        <v>-2.34</v>
+        <v>-2.26</v>
       </c>
       <c r="F31" s="1">
-        <v>-2.34</v>
+        <v>-2.26</v>
       </c>
       <c r="G31" s="1">
-        <v>-2.33</v>
+        <v>-2.26</v>
       </c>
       <c r="H31" s="1">
-        <v>-2.33</v>
+        <v>-2.26</v>
       </c>
       <c r="I31" s="1">
-        <v>-2.32</v>
+        <v>-2.26</v>
       </c>
       <c r="J31" s="1">
-        <v>-2.32</v>
+        <v>-2.26</v>
       </c>
       <c r="K31" s="1">
-        <v>-2.32</v>
+        <v>-2.27</v>
       </c>
       <c r="L31" s="1">
-        <v>-2.32</v>
+        <v>-2.27</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -1126,37 +1119,37 @@
         <v>14</v>
       </c>
       <c r="B32" s="1">
-        <v>22.91</v>
+        <v>26.85</v>
       </c>
       <c r="C32" s="1">
-        <v>21.04</v>
+        <v>26.25</v>
       </c>
       <c r="D32" s="1">
-        <v>8.140000000000001</v>
+        <v>9.720000000000001</v>
       </c>
       <c r="E32" s="1">
-        <v>8.539999999999999</v>
+        <v>8.789999999999999</v>
       </c>
       <c r="F32" s="1">
-        <v>8.369999999999999</v>
+        <v>8.789999999999999</v>
       </c>
       <c r="G32" s="1">
-        <v>6.53</v>
+        <v>8.17</v>
       </c>
       <c r="H32" s="1">
-        <v>6.12</v>
+        <v>7.67</v>
       </c>
       <c r="I32" s="1">
-        <v>6.09</v>
+        <v>7.78</v>
       </c>
       <c r="J32" s="1">
-        <v>6.51</v>
+        <v>8.09</v>
       </c>
       <c r="K32" s="1">
-        <v>6.38</v>
+        <v>7.91</v>
       </c>
       <c r="L32" s="1">
-        <v>5.65</v>
+        <v>8.01</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -1169,37 +1162,37 @@
         <v>20</v>
       </c>
       <c r="B35" s="1">
-        <v>14.82</v>
+        <v>15.13</v>
       </c>
       <c r="C35" s="1">
-        <v>14.99</v>
+        <v>15.38</v>
       </c>
       <c r="D35" s="1">
-        <v>14.88</v>
+        <v>14.71</v>
       </c>
       <c r="E35" s="1">
-        <v>15.49</v>
+        <v>15.09</v>
       </c>
       <c r="F35" s="1">
-        <v>15.45</v>
+        <v>15.09</v>
       </c>
       <c r="G35" s="1">
+        <v>15.03</v>
+      </c>
+      <c r="H35" s="1">
+        <v>15.09</v>
+      </c>
+      <c r="I35" s="1">
+        <v>15.12</v>
+      </c>
+      <c r="J35" s="1">
+        <v>15.17</v>
+      </c>
+      <c r="K35" s="1">
+        <v>15.17</v>
+      </c>
+      <c r="L35" s="1">
         <v>15.21</v>
-      </c>
-      <c r="H35" s="1">
-        <v>15.28</v>
-      </c>
-      <c r="I35" s="1">
-        <v>15.29</v>
-      </c>
-      <c r="J35" s="1">
-        <v>15.37</v>
-      </c>
-      <c r="K35" s="1">
-        <v>15.4</v>
-      </c>
-      <c r="L35" s="1">
-        <v>15.28</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -1207,37 +1200,37 @@
         <v>21</v>
       </c>
       <c r="B36" s="1">
-        <v>20.18</v>
+        <v>19.85</v>
       </c>
       <c r="C36" s="1">
-        <v>20.83</v>
+        <v>20.39</v>
       </c>
       <c r="D36" s="1">
-        <v>23.57</v>
+        <v>23.09</v>
       </c>
       <c r="E36" s="1">
-        <v>24.4</v>
+        <v>23.78</v>
       </c>
       <c r="F36" s="1">
-        <v>24.36</v>
+        <v>23.78</v>
       </c>
       <c r="G36" s="1">
-        <v>24.26</v>
+        <v>23.78</v>
       </c>
       <c r="H36" s="1">
-        <v>24.41</v>
+        <v>23.93</v>
       </c>
       <c r="I36" s="1">
-        <v>24.43</v>
+        <v>23.96</v>
       </c>
       <c r="J36" s="1">
-        <v>24.49</v>
+        <v>24</v>
       </c>
       <c r="K36" s="1">
-        <v>24.55</v>
+        <v>24.02</v>
       </c>
       <c r="L36" s="1">
-        <v>24.48</v>
+        <v>24.06</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -1245,37 +1238,37 @@
         <v>22</v>
       </c>
       <c r="B37" s="1">
-        <v>27.4</v>
+        <v>27.11</v>
       </c>
       <c r="C37" s="1">
-        <v>27.6</v>
+        <v>27.1</v>
       </c>
       <c r="D37" s="1">
-        <v>30.93</v>
+        <v>30.44</v>
       </c>
       <c r="E37" s="1">
-        <v>31.03</v>
+        <v>30.42</v>
       </c>
       <c r="F37" s="1">
-        <v>30.96</v>
+        <v>30.38</v>
       </c>
       <c r="G37" s="1">
-        <v>30.78</v>
+        <v>30.3</v>
       </c>
       <c r="H37" s="1">
-        <v>30.79</v>
+        <v>30.29</v>
       </c>
       <c r="I37" s="1">
-        <v>30.82</v>
+        <v>30.3</v>
       </c>
       <c r="J37" s="1">
-        <v>30.86</v>
+        <v>30.34</v>
       </c>
       <c r="K37" s="1">
-        <v>30.91</v>
+        <v>30.35</v>
       </c>
       <c r="L37" s="1">
-        <v>30.84</v>
+        <v>30.38</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -1283,37 +1276,37 @@
         <v>23</v>
       </c>
       <c r="B38" s="1">
-        <v>6.91</v>
+        <v>8.279999999999999</v>
       </c>
       <c r="C38" s="1">
-        <v>6.21</v>
+        <v>8.039999999999999</v>
       </c>
       <c r="D38" s="1">
-        <v>0.5</v>
+        <v>0.96</v>
       </c>
       <c r="E38" s="1">
-        <v>0.59</v>
+        <v>0.68</v>
       </c>
       <c r="F38" s="1">
-        <v>0.54</v>
+        <v>0.67</v>
       </c>
       <c r="G38" s="1">
-        <v>0.04</v>
+        <v>0.51</v>
       </c>
       <c r="H38" s="1">
-        <v>-0.07000000000000001</v>
+        <v>0.37</v>
       </c>
       <c r="I38" s="1">
-        <v>-0.07000000000000001</v>
+        <v>0.4</v>
       </c>
       <c r="J38" s="1">
-        <v>0.04</v>
+        <v>0.48</v>
       </c>
       <c r="K38" s="1">
-        <v>0</v>
+        <v>0.43</v>
       </c>
       <c r="L38" s="1">
-        <v>-0.19</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -1335,11 +1328,6 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
-      <c r="A43" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
     <row r="45" spans="1:12">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
@@ -1355,12 +1343,6 @@
       <c r="L45" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B12:L38">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
-      <formula>0.001</formula>
-      <formula>0.049</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>